<commit_message>
Temporary commit before filter-branch
</commit_message>
<xml_diff>
--- a/pdbanalysis/aukb_wt_125256.xlsx
+++ b/pdbanalysis/aukb_wt_125256.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonhwang/Documents/Brown/Rubenstein/pdbanalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCC59992-EFDD-F541-A4A3-D4E22D5A9ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE789B69-17CF-7149-B08C-C79A70BD7482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14940" xr2:uid="{30C6DF77-5CE0-7149-B0BE-B6D3ECE09662}"/>
+    <workbookView xWindow="1000" yWindow="660" windowWidth="27240" windowHeight="14940" xr2:uid="{30C6DF77-5CE0-7149-B0BE-B6D3ECE09662}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,170 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_041_alphafold2_ptm_model_2_seed_003</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_001_alphafold2_ptm_model_1_seed_002</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_029_alphafold2_ptm_model_4_seed_008</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_049_alphafold2_ptm_model_5_seed_008</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_009_alphafold2_ptm_model_2_seed_002</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_042_alphafold2_ptm_model_3_seed_000</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_019_alphafold2_ptm_model_4_seed_003</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_015_alphafold2_ptm_model_4_seed_000</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_046_alphafold2_ptm_model_3_seed_009</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_021_alphafold2_ptm_model_1_seed_009</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_031_alphafold2_ptm_model_5_seed_007</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_032_alphafold2_ptm_model_4_seed_006</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_003_alphafold2_ptm_model_2_seed_004</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_043_alphafold2_ptm_model_3_seed_008</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_048_alphafold2_ptm_model_3_seed_004</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_017_alphafold2_ptm_model_4_seed_009</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_018_alphafold2_ptm_model_1_seed_000</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_034_alphafold2_ptm_model_5_seed_002</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_038_alphafold2_ptm_model_3_seed_001</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_020_alphafold2_ptm_model_2_seed_009</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_010_alphafold2_ptm_model_2_seed_001</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_004_alphafold2_ptm_model_2_seed_008</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_044_alphafold2_ptm_model_3_seed_007</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_028_alphafold2_ptm_model_4_seed_004</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_047_alphafold2_ptm_model_5_seed_006</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_027_alphafold2_ptm_model_4_seed_007</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_008_alphafold2_ptm_model_1_seed_008</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_037_alphafold2_ptm_model_1_seed_003</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_040_alphafold2_ptm_model_5_seed_003</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_023_alphafold2_ptm_model_4_seed_002</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_030_alphafold2_ptm_model_5_seed_005</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_013_alphafold2_ptm_model_1_seed_006</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_014_alphafold2_ptm_model_2_seed_006</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_007_alphafold2_ptm_model_4_seed_001</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_033_alphafold2_ptm_model_5_seed_000</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_024_alphafold2_ptm_model_1_seed_007</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_050_alphafold2_ptm_model_3_seed_006</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_016_alphafold2_ptm_model_1_seed_004</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_002_alphafold2_ptm_model_2_seed_005</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_012_alphafold2_ptm_model_4_seed_005</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_045_alphafold2_ptm_model_3_seed_002</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_005_alphafold2_ptm_model_1_seed_005</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_006_alphafold2_ptm_model_1_seed_001</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_025_alphafold2_ptm_model_2_seed_000</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_022_alphafold2_ptm_model_5_seed_009</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_011_alphafold2_ptm_model_2_seed_007</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_036_alphafold2_ptm_model_5_seed_004</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_026_alphafold2_ptm_model_3_seed_005</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_035_alphafold2_ptm_model_5_seed_001</t>
+  </si>
+  <si>
+    <t>aukb_domain_wt_unrelaxed_rank_039_alphafold2_ptm_model_3_seed_003</t>
+  </si>
+  <si>
+    <t>G loop</t>
+  </si>
+  <si>
+    <t>DFG</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -44,13 +205,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -65,8 +240,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,12 +560,576 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86164C8B-3DF2-4146-83DB-7708A297A282}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="86.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.83375388383865301</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2.7962229251861501</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.81948769092559803</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.8238217830657901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.85279810428619296</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2.8347523212432799</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.80964481830596902</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2.8299319744110099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.83718794584274203</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2.8222908973693799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.85113745927810602</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2.8314847946166899</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.86110103130340498</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2.7909662723541202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.82110440731048495</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2.81313896179199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.82452249526977495</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2.8151586055755602</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.86125677824020297</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2.8366055488586399</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.84165787696838301</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2.8018591403961102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.84509599208831698</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2.7944488525390598</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.85313332080840998</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2.8490698337554901</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.84960848093032804</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2.84087657928466</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.87531501054763705</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2.8004350662231401</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.863081455230712</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2.8348801136016801</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.875585317611694</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2.81895422935485</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.851518213748931</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2.82270312309265</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.85378104448318404</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2.78397536277771</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.83761292695999101</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2.8465564250946001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.83212625980377197</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2.8444135189056299</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.89055204391479403</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2.8163375854492099</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.88089531660079901</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2.77683401107788</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.83195191621780396</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2.8187389373779199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.844476819038391</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2.8098759651184002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27">
+        <v>0.92302101850509599</v>
+      </c>
+      <c r="C27">
+        <v>2.8184843063354399</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>0.85731619596481301</v>
+      </c>
+      <c r="C28">
+        <v>2.76646423339843</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29">
+        <v>0.89583843946456898</v>
+      </c>
+      <c r="C29">
+        <v>2.79708528518676</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>0.83611989021301203</v>
+      </c>
+      <c r="C30">
+        <v>2.7969505786895699</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>1.0108352899551301</v>
+      </c>
+      <c r="C31">
+        <v>2.7703390121459899</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32">
+        <v>0.95114541053771895</v>
+      </c>
+      <c r="C32">
+        <v>2.7676928043365399</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0.876057147979736</v>
+      </c>
+      <c r="C33" s="2">
+        <v>2.7799913883209202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34">
+        <v>1.03400695323944</v>
+      </c>
+      <c r="C34">
+        <v>2.78698301315307</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35">
+        <v>0.97523438930511397</v>
+      </c>
+      <c r="C35">
+        <v>2.7508573532104399</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36">
+        <v>0.95838207006454401</v>
+      </c>
+      <c r="C36">
+        <v>2.74720883369445</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37">
+        <v>1.07428073883056</v>
+      </c>
+      <c r="C37">
+        <v>2.7907176017761199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0.84604769945144598</v>
+      </c>
+      <c r="C38" s="2">
+        <v>2.83005690574646</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39">
+        <v>0.93420833349227905</v>
+      </c>
+      <c r="C39">
+        <v>2.7828772068023602</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40">
+        <v>0.95307523012161199</v>
+      </c>
+      <c r="C40">
+        <v>2.7906525135040199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41">
+        <v>1.0419833660125699</v>
+      </c>
+      <c r="C41">
+        <v>2.7830970287322998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>0.87058818340301503</v>
+      </c>
+      <c r="C42">
+        <v>2.82077956199646</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>0.94322425127029397</v>
+      </c>
+      <c r="C43">
+        <v>2.8076605796813898</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44">
+        <v>0.93709456920623702</v>
+      </c>
+      <c r="C44">
+        <v>2.8300192356109601</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45">
+        <v>0.95810842514037997</v>
+      </c>
+      <c r="C45">
+        <v>2.80244660377502</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46">
+        <v>1.0847851037979099</v>
+      </c>
+      <c r="C46">
+        <v>2.79355716705322</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47">
+        <v>1.02422106266021</v>
+      </c>
+      <c r="C47">
+        <v>2.82594442367553</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48">
+        <v>0.98101806640625</v>
+      </c>
+      <c r="C48">
+        <v>2.7870349884033199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49">
+        <v>0.93290334939956598</v>
+      </c>
+      <c r="C49">
+        <v>2.8318171501159601</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50">
+        <v>1.00848424434661</v>
+      </c>
+      <c r="C50">
+        <v>2.7886276245117099</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51">
+        <v>0.95320445299148504</v>
+      </c>
+      <c r="C51">
+        <v>2.8564214706420898</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>